<commit_message>
Tesl Llama for binary predictions
</commit_message>
<xml_diff>
--- a/data/xcellent-sentences.xlsx
+++ b/data/xcellent-sentences.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\apavlyuchenko\Documents\Projects\ContentAnalysis\SemanticDifferentialNLP\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4679B213-076D-46AD-B9EA-1BC09B80C9F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB80C63B-E441-482D-9699-4EB7B8CF80BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4426857C-0242-4E4E-8A69-B645C4B17CDB}"/>
   </bookViews>
@@ -1154,7 +1154,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9EFA7F8-E661-499E-923B-DCD03E4444EF}">
   <dimension ref="A1:E240"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C94" sqref="C94"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2089,13 +2091,13 @@
         <v>243</v>
       </c>
       <c r="C55">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D55" t="s">
         <v>245</v>
       </c>
       <c r="E55" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -2752,7 +2754,7 @@
         <v>243</v>
       </c>
       <c r="C94">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D94" t="s">
         <v>245</v>

</xml_diff>